<commit_message>
output to excel done
</commit_message>
<xml_diff>
--- a/my-diff-2.xlsx
+++ b/my-diff-2.xlsx
@@ -59,9 +59,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -362,7 +365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -371,6 +374,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>PAYMENT_ID</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>CONTRACT_NO</t>
@@ -408,149 +416,137 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>PAYMENT_ID</t>
+          <t>FX_Rate</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>FX_Rate</t>
+          <t>Cost (USD)</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Cost (USD)</t>
+          <t>Cost (Local)</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Cost (Local)</t>
+          <t>Approval_date</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Approval_date</t>
+          <t>Approver_Name</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Approver_Name</t>
+          <t>Cash_localAmt</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Cash_localAmt</t>
+          <t>Cash_deducted_amt</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Cash_deducted_amt</t>
+          <t>Cash_USDAmt</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Cash_USDAmt</t>
+          <t>Balance_Payment_Local</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Balance_Payment_Local</t>
+          <t>Balance_Payment_USD</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Balance_Payment_USD</t>
+          <t>Payment_Received_Date</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Payment_Received_Date</t>
+          <t>Issue_Date</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Issue_Date</t>
+          <t>Last_UpdatedDate</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Last_UpdatedDate</t>
+          <t>Payment_Comments</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Payment_Comments</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
           <t>Products</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>version</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>12529</v>
-      </c>
-      <c r="C2" t="inlineStr">
+        <v>12443</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>100021</v>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">VAT INVOICE </t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>GBP</t>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Contract Modification - Advance</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>USD</t>
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>38001</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Partial</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>AVAINV56</t>
-        </is>
+        <v>37516</v>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6197</v>
+        <v>30000</v>
       </c>
       <c r="K2" t="n">
-        <v>113.77</v>
-      </c>
-      <c r="L2" t="n">
-        <v>70.5</v>
-      </c>
-      <c r="M2" s="2" t="n">
-        <v>38007</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Test3</t>
-        </is>
+        <v>30000</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>37532</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>TEST 1 ---&gt; TEST1</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>30000</v>
       </c>
       <c r="O2" t="n">
-        <v>70.5</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -561,87 +557,85 @@
       <c r="R2" t="n">
         <v>0</v>
       </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2" t="n">
-        <v>38001</v>
-      </c>
-      <c r="U2" s="2" t="n">
-        <v>38007</v>
-      </c>
-      <c r="V2" t="inlineStr"/>
+      <c r="S2" s="3" t="n">
+        <v>37516</v>
+      </c>
+      <c r="T2" s="3" t="n">
+        <v>37532</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>NaT ---&gt; NaT</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">contact someone from your SAP team to adjust the setting. This setting ??? can only be adjusted in your SAP development system and transported through your system landscape. ---&gt; contact someone from your SAP team to adjust the setting. This setting ???         can only be adjusted in your SAP development system and transported through your system landscape.      </t>
+        </is>
+      </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t xml:space="preserve">contact someone from your SAP team to adjust the setting. This setting ??? can only be adjusted in your SAP development system and transported through your system landscape.    </t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>old</t>
+          <t>Caps, αSportsKit, Shóes, ?T-Shirts,  ---&gt; Shóes, ?T-Shirts, Caps, αSportsKit</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
+        <v>12444</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>100021</v>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>Royalty Jul 16-Sep 16/G4-4</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>37561</v>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>Confirmed</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>12529</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">VAT INVOICE </t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>38001</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Partial</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>AVAINV67</t>
-        </is>
-      </c>
       <c r="J3" t="n">
-        <v>0.6197</v>
+        <v>90000</v>
       </c>
       <c r="K3" t="n">
-        <v>246.52</v>
-      </c>
-      <c r="L3" t="n">
-        <v>152.76</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>38007</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Test3</t>
-        </is>
+        <v>90000</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>37532</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>TEST-1 ---&gt; TEST1</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>90000</v>
       </c>
       <c r="O3" t="n">
-        <v>152.76</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
         <v>0</v>
@@ -652,81 +646,85 @@
       <c r="R3" t="n">
         <v>0</v>
       </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2" t="n">
-        <v>38001</v>
-      </c>
-      <c r="U3" s="2" t="n">
-        <v>38007</v>
-      </c>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>old</t>
+      <c r="S3" s="3" t="n">
+        <v>37561</v>
+      </c>
+      <c r="T3" s="3" t="n">
+        <v>37532</v>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>NaT ---&gt; NaT</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Cleared/</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>software product, computer game, book, videogame, magaziñe or other publication, souñd recording, video recording,   ---&gt; book, magaziñe or other publication, souñd recording, video recording, software product, computer game, videogame,</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>12529</v>
-      </c>
-      <c r="C4" t="inlineStr">
+        <v>12445</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>100023</v>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">VAT INVOICE </t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>GBP</t>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>VAT @ 5.000000.00%</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>USD</t>
         </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>38001</v>
-      </c>
-      <c r="G4" t="n">
+        <v>37742</v>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>Unpaid</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
         <v>1</v>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Partial</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>AVAINV56</t>
-        </is>
-      </c>
       <c r="J4" t="n">
-        <v>0.6197</v>
+        <v>90000</v>
       </c>
       <c r="K4" t="n">
-        <v>113.77</v>
-      </c>
-      <c r="L4" t="n">
-        <v>70.5</v>
-      </c>
-      <c r="M4" s="2" t="n">
-        <v>38007</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Test3</t>
-        </is>
+        <v>90000</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>37532</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>TEST2</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>90000</v>
       </c>
       <c r="O4" t="n">
-        <v>70.5</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
@@ -737,46 +735,48 @@
       <c r="R4" t="n">
         <v>0</v>
       </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" s="2" t="n">
-        <v>38001</v>
-      </c>
-      <c r="U4" s="2" t="n">
-        <v>38007</v>
-      </c>
-      <c r="V4" t="inlineStr"/>
+      <c r="S4" s="3" t="n">
+        <v>37742</v>
+      </c>
+      <c r="T4" s="3" t="n">
+        <v>37532</v>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>NaT ---&gt; NaT</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>nan ---&gt; nan</t>
+        </is>
+      </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t xml:space="preserve">contact someone from your SAP team to adjust the setting. This setting ??? can only be adjusted in your SAP development system and transported through your system landscape.    </t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>new</t>
+          <t>sound recording, video recording, book, magazine or other publication          ---&gt; book, magazine or other publication, sound recording, video recording</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>AVAINV23</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>12529</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">VAT INVOICE </t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>VAT Tax for June 2003</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>GBP</t>
         </is>
@@ -784,38 +784,40 @@
       <c r="F5" s="2" t="n">
         <v>38001</v>
       </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="inlineStr">
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
         <is>
           <t>Partial</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>AVAINV67</t>
-        </is>
+      <c r="I5" t="n">
+        <v>0.6197</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6197</v>
+        <v>568.86</v>
       </c>
       <c r="K5" t="n">
-        <v>246.52</v>
-      </c>
-      <c r="L5" t="n">
-        <v>152.76</v>
-      </c>
-      <c r="M5" s="2" t="n">
+        <v>352.5</v>
+      </c>
+      <c r="L5" s="3" t="n">
         <v>38007</v>
       </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Test3</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Test3</t>
+          <t>-352.5 ---&gt; -300.95</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>152.76</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
@@ -826,21 +828,25 @@
       <c r="R5" t="n">
         <v>0</v>
       </c>
-      <c r="S5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2" t="n">
+      <c r="S5" s="3" t="n">
         <v>38001</v>
       </c>
-      <c r="U5" s="2" t="n">
+      <c r="T5" s="3" t="n">
         <v>38007</v>
       </c>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>new</t>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>NaT ---&gt; NaT</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>nan ---&gt; nan</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>nan ---&gt; nan</t>
         </is>
       </c>
     </row>

</xml_diff>